<commit_message>
Changes for lecture 2
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B7485F-6B5E-5A44-B2F0-E78D3CD21D46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FAF3DA-6015-A94B-BE7B-C3EC2DFF470C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="4560" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>withinWeek</t>
   </si>
   <si>
-    <t>Uninformed Search (BFS, DFS, IDS)</t>
-  </si>
-  <si>
     <t>Hill Climbers, Simulated Annealing</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Hill Climbers Lab</t>
   </si>
   <si>
-    <t>PA 1; HW 1; Quiz 1</t>
-  </si>
-  <si>
     <t>PA 0</t>
   </si>
   <si>
@@ -272,6 +266,12 @@
   </si>
   <si>
     <t>What is AI;Intel Agents; slides(slides/01_IntroAndAgents.pdf)</t>
+  </si>
+  <si>
+    <t>Uninformed Search (BFS, DFS, IDS);slides(slides/02_UninformedSearch)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>PA 1; HW 1; Quiz 0</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1542B99F-AEAE-5746-AE3C-5BDDA5FB5C77}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -690,13 +690,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -710,17 +710,17 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -734,14 +734,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -755,17 +755,17 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -779,11 +779,11 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -797,14 +797,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2"/>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -833,14 +833,14 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3"/>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -869,11 +869,11 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3"/>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -902,11 +902,11 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3"/>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -920,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -934,10 +934,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -965,10 +965,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1103,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1131,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1159,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1193,130 +1193,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
         <v>66</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move PA1 due date
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC094B6C-1556-7A4A-97B0-1E6942D9BE73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B4D0C1DE-12E5-C44E-8539-94A428E8D266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="4560" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>week</t>
   </si>
@@ -109,9 +109,6 @@
     <t>HW 3</t>
   </si>
   <si>
-    <t>HW4; PA2</t>
-  </si>
-  <si>
     <t>Assessment Day - No Class</t>
   </si>
   <si>
@@ -157,15 +154,9 @@
     <t>Quiz 3</t>
   </si>
   <si>
-    <t>PA 2; Quiz 4</t>
-  </si>
-  <si>
     <t>Review/Muddiest Points</t>
   </si>
   <si>
-    <t>PA 2; Quiz 6</t>
-  </si>
-  <si>
     <t>Quiz 5</t>
   </si>
   <si>
@@ -175,12 +166,6 @@
     <t>HW 0 (hw/hw0.php); PA 0 (PAs/PA.php?paNumber=0)</t>
   </si>
   <si>
-    <t>HW 2 (hw/hw2.php; PA 2 (PAS/PA.php?paNumber=2)</t>
-  </si>
-  <si>
-    <t>HW 3 (hw/hw3.php)</t>
-  </si>
-  <si>
     <t>Chp 4.1</t>
   </si>
   <si>
@@ -265,10 +250,10 @@
     <t>Uninformed Search (BFS, DFS, IDS);slides(slides/02_UninformedSearch)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
-    <t>PA 1; HW 1; Quiz 0</t>
-  </si>
-  <si>
     <t>HW 1 (hw/hw1.php); PA 1(PAs/PA.php?paNumber=1)</t>
+  </si>
+  <si>
+    <t>HW 2;Quiz 0</t>
   </si>
 </sst>
 </file>
@@ -637,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1542B99F-AEAE-5746-AE3C-5BDDA5FB5C77}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,13 +668,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -703,16 +688,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -729,10 +714,13 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -749,13 +737,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -769,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -792,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -806,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -821,12 +809,6 @@
       </c>
       <c r="D9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -840,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -856,9 +838,6 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -885,10 +864,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -902,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -916,10 +892,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -933,10 +906,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -947,13 +920,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -967,7 +937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
@@ -981,7 +951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
@@ -995,7 +965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1009,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1020,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1034,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1045,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1056,10 +1026,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1070,10 +1040,10 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1084,10 +1054,10 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1098,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1112,10 +1082,10 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1126,10 +1096,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1140,10 +1110,10 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>
@@ -1174,26 +1144,26 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1201,103 +1171,103 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slides for lecture3 and a few mods to PA01
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5947E4F1-51B8-344D-B43B-6B7BE43DD0D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9AFEF3-95CA-7D41-A4C8-6953E8F9C1EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="4560" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="8560" yWindow="4720" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -100,12 +100,6 @@
     <t>slack</t>
   </si>
   <si>
-    <t>Informed Search(A*, Graph Search)</t>
-  </si>
-  <si>
-    <t>HW 2</t>
-  </si>
-  <si>
     <t>HW 3</t>
   </si>
   <si>
@@ -250,10 +244,16 @@
     <t>Uninformed Search (BFS, DFS, IDS);slides(slides/02_UninformedSearch)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
-    <t>HW 1 (hw/hw1.php); PA 1(PAs/PA.php?paNumber=1)</t>
-  </si>
-  <si>
-    <t>PA 1;HW 2;Quiz 0</t>
+    <t>HW 2;Quiz 0</t>
+  </si>
+  <si>
+    <t>HW 1 (https://canvas.jmu.edu/courses/1775272/quizzes); PA 1(PAs/PA.php?paNumber=1)</t>
+  </si>
+  <si>
+    <t>HW 2 (https://canvas.jmu.edu/courses/1775272/quizzes)</t>
+  </si>
+  <si>
+    <t>Informed Search = A* and Graph Search;slides(slides/03_03_InformedSearch.pdf)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,13 +668,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -688,16 +688,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -711,16 +711,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -737,13 +737,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -757,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -864,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -892,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1026,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1068,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1110,7 +1110,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1144,130 +1144,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix yet another calendar typo
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E825825-4231-D24C-B1D9-A20EF90254F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FF0F2C-2BC1-9A48-B2DE-9B95625237C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8560" yWindow="4720" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
@@ -241,9 +241,6 @@
     <t>What is AI;Intel Agents; slides(slides/01_IntroAndAgents.pdf)</t>
   </si>
   <si>
-    <t>Uninformed Search (BFS, DFS, IDS);slides(slides/02_UninformedSearch)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
-  </si>
-  <si>
     <t>HW 2;Quiz 0</t>
   </si>
   <si>
@@ -253,7 +250,10 @@
     <t>HW 2 (https://canvas.jmu.edu/courses/1775272/quizzes)</t>
   </si>
   <si>
-    <t>Informed Search = A* and Graph Search;slides(slides/03_InformedSearch.pdf)   video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+    <t>Uninformed Search (BFS, DFS, IDS);slides(slides/02_UninformedSearch)  ; video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Informed Search = A* and Graph Search;slides(slides/03_InformedSearch.pdf) ;video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,13 +688,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -717,7 +717,7 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
         <v>46</v>
@@ -743,7 +743,7 @@
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to Calendar and notes on quiz 1 Slides for Lecture 5
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C61829E6-8452-3442-BCD7-FD6228580879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C03AC453-9428-A14E-B6A0-28CDC163ADCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42260" yWindow="3960" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="-35620" yWindow="3900" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>week</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Chp 1, Chp 2</t>
   </si>
   <si>
-    <t>CSPs 1</t>
-  </si>
-  <si>
     <t>CSPs 2</t>
   </si>
   <si>
@@ -257,6 +254,18 @@
   </si>
   <si>
     <t>Chp 6.1 - 6.3</t>
+  </si>
+  <si>
+    <t>Chp 6.4 - 6.5</t>
+  </si>
+  <si>
+    <t>PA 2; HW 3</t>
+  </si>
+  <si>
+    <t>CSPs Part 1; slides(slides/0505_CSP_Part1.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Quiz 0 Retake;Quiz 1(mquizzes/mquiz1/mquiz1.php)</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -691,16 +700,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -714,16 +723,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -737,16 +746,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -760,10 +769,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -776,17 +785,17 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
+      <c r="D7" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -800,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,7 +823,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -828,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -870,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -884,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -898,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -912,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -926,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -940,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -954,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -968,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -982,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1032,7 +1047,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1046,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1060,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1088,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1102,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1116,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1130,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1150,130 +1165,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lecture 6 and calendar updates
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EA5452-123E-194A-A585-2ED33367460E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46A5F977-FF26-744D-8E78-3A3D834AFB3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35620" yWindow="3900" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="-41140" yWindow="4500" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>week</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Heuristic Alpha/Beta Search, Monte Carlo Search, Chance Trees</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>MDP</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Chp 1, Chp 2</t>
   </si>
   <si>
-    <t>CSPs 2</t>
-  </si>
-  <si>
     <t>Prop Logic (Theorem Proving)</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>Quiz 5</t>
   </si>
   <si>
-    <t>CSP Lab</t>
-  </si>
-  <si>
     <t>HW 0 (hw/hw0.php); PA 0 (PAs/PA.php?paNumber=0)</t>
   </si>
   <si>
@@ -256,16 +247,34 @@
     <t>Chp 6.4 - 6.5</t>
   </si>
   <si>
-    <t>PA 2; HW 3</t>
-  </si>
-  <si>
-    <t>Quiz 0 Retake;Quiz 1(mquizzes/mquiz1/mquiz1.php)</t>
-  </si>
-  <si>
     <t>CSPs Part 1; slides(slides/05_CSP_Part1.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
     <t>Uninformed Search BFS, DFS, IDS;slides(slides/02_UninformedSearch.pdf)  ; video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>CSPs Part 2; slides(slides/06_CSP_Part2.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>HW 3(https://canvas.jmu.edu/courses/1775272/quizzes)</t>
+  </si>
+  <si>
+    <t>HW4(https://canvas.jmu.edu/courses/1775272/quizzes)</t>
+  </si>
+  <si>
+    <t>Quiz 0 Retake;</t>
+  </si>
+  <si>
+    <t>HW4;Quiz 1(mquizzes/mquiz1/mquiz1.php)</t>
+  </si>
+  <si>
+    <t>Chance Tree Lab</t>
+  </si>
+  <si>
+    <t>Chp 5.1 - 5.4</t>
+  </si>
+  <si>
+    <t>Chp 5.5 - 5.7</t>
   </si>
 </sst>
 </file>
@@ -634,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1542B99F-AEAE-5746-AE3C-5BDDA5FB5C77}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,13 +689,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -700,16 +709,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -723,16 +732,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -746,16 +755,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -769,10 +778,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -786,16 +795,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
         <v>75</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -809,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -823,13 +832,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -843,7 +855,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -857,7 +872,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -871,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -885,7 +903,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -899,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -913,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -927,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -941,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -955,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -969,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -983,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -997,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1022,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1047,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1061,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1075,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1089,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1103,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1117,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1131,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1145,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1165,130 +1183,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add PA2 notes and slides from Lecture 7.
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46A5F977-FF26-744D-8E78-3A3D834AFB3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389C586-2040-0849-B2C9-EA4367C20819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41140" yWindow="4500" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="10520" yWindow="3700" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>week</t>
   </si>
@@ -58,9 +58,6 @@
     <t>withinWeek</t>
   </si>
   <si>
-    <t>Adversarial Search -- Alpha/Beta Pruning</t>
-  </si>
-  <si>
     <t>Heuristic Alpha/Beta Search, Monte Carlo Search, Chance Trees</t>
   </si>
   <si>
@@ -275,6 +272,15 @@
   </si>
   <si>
     <t>Chp 5.5 - 5.7</t>
+  </si>
+  <si>
+    <t>Adversarial Search -- Alpha/Beta Pruning;slides(slides/07_AdversarialSearch.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>HW5(https://canvas.jmu.edu/courses/1775272/quizzes)</t>
+  </si>
+  <si>
+    <t>Quiz 2(mquizzes/mquiz2/mquiz2.php)</t>
   </si>
 </sst>
 </file>
@@ -644,7 +650,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,13 +695,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -709,16 +715,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -732,16 +738,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -755,16 +761,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -778,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -795,16 +801,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
         <v>74</v>
-      </c>
-      <c r="G7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -818,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -832,16 +838,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -855,10 +861,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -872,10 +881,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -889,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -903,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -917,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -931,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -945,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -959,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -973,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -987,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1001,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1040,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1065,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1079,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1093,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1107,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1121,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1135,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1149,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1163,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1183,130 +1195,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expectimax and utility slides and calendar update.
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A9A4BAB-1DF5-A647-8F6F-1FB569149F98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF78E17-9FDD-0840-8834-09AA04248755}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10520" yWindow="3700" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="-41500" yWindow="5600" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>withinWeek</t>
   </si>
   <si>
-    <t>Heuristic Alpha/Beta Search, Monte Carlo Search, Chance Trees</t>
-  </si>
-  <si>
     <t>MDP</t>
   </si>
   <si>
@@ -271,19 +268,22 @@
     <t>Chp 5.1 - 5.4</t>
   </si>
   <si>
-    <t>Chp 5.5 - 5.7</t>
-  </si>
-  <si>
     <t>Adversarial Search -- Alpha/Beta Pruning;slides(slides/07_AdversarialSearch.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
     <t>HW5(https://canvas.jmu.edu/courses/1775272/quizzes)</t>
   </si>
   <si>
-    <t>Quiz 2(mquizzes/mquiz2/mquiz2.php)</t>
-  </si>
-  <si>
     <t>PA 2  (PAs/PA.php?paNumber=2)</t>
+  </si>
+  <si>
+    <t>Chp 5.5 - 5.7; Chp 16.1 - 16.3</t>
+  </si>
+  <si>
+    <t>Expectimax, Utility Functions;slides(slides/08_ExpectimaxSearch.pdf);video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Quiz 1 Retake;Quiz 2(mquizzes/mquiz2/mquiz2.php)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,13 +698,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,16 +718,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -741,16 +741,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -764,16 +764,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -801,16 +801,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
         <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -824,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -838,16 +838,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -861,13 +861,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -881,13 +881,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -915,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1052,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1105,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1195,130 +1195,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RL material and calendar updates
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C564FA3-5E41-2144-A880-562BE1D9A3A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459A68BB-C41B-F140-B3EE-B2C38A7B601A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48600" yWindow="2700" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="9940" yWindow="3660" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>week</t>
   </si>
@@ -67,12 +67,6 @@
     <t>Chp 1, Chp 2</t>
   </si>
   <si>
-    <t>Prop Logic (Theorem Proving)</t>
-  </si>
-  <si>
-    <t>Agents using Prop Logic</t>
-  </si>
-  <si>
     <t>FOL, Unification</t>
   </si>
   <si>
@@ -103,12 +97,6 @@
     <t>Hidden Markov Models</t>
   </si>
   <si>
-    <t>Reinforcement Learning 1</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning 2</t>
-  </si>
-  <si>
     <t>Bayes - Representations</t>
   </si>
   <si>
@@ -274,9 +262,6 @@
     <t>Quiz 1 Retake;Quiz 2(mquizzes/mquiz2/mquiz2.php)</t>
   </si>
   <si>
-    <t>Chp 17.1-17.3</t>
-  </si>
-  <si>
     <t>HW6(https://canvas.jmu.edu/courses/1775272/quizzes)</t>
   </si>
   <si>
@@ -286,13 +271,46 @@
     <t>Chp 22</t>
   </si>
   <si>
-    <t>Chance Tree Lab;Review/Muddiest Points; video(https://canvas.jmu.edu/courses/1775272/modules)</t>
-  </si>
-  <si>
     <t>Markov Decision Processes 1;slides(slides/09_MDP_Part1.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
     <t>Markov Decision Processes 2;slides(slides/10_MDP_Part2.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Review/Muddiest Points; video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Chance Tree Lab; video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Chp 17.3</t>
+  </si>
+  <si>
+    <t>Chp 17.1 - 17.2</t>
+  </si>
+  <si>
+    <t>Quiz 3(mquizzes/mquiz3/mquiz3.php)</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning 1;slides(slides/11_RL_Part1.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning 2;slides(slides/12_RL_Part2.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Proposition Logic and Logical Agents</t>
+  </si>
+  <si>
+    <t>Chp 7.1-7.4</t>
+  </si>
+  <si>
+    <t>Theorm Proving and Resolution</t>
+  </si>
+  <si>
+    <t>Chp 7.5</t>
   </si>
 </sst>
 </file>
@@ -661,13 +679,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1542B99F-AEAE-5746-AE3C-5BDDA5FB5C77}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="73.83203125" customWidth="1"/>
+    <col min="4" max="4" width="118.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
@@ -707,13 +725,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -727,16 +745,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -750,16 +768,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -773,16 +791,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -796,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -810,16 +828,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>69</v>
-      </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -833,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -847,16 +865,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
         <v>67</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -870,13 +888,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -890,13 +908,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -910,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -924,16 +942,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -947,7 +962,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -961,10 +979,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -978,10 +999,16 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -992,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1006,10 +1033,13 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1020,10 +1050,13 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1034,10 +1067,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1047,8 +1080,11 @@
       <c r="C21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1062,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1073,7 +1109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1084,10 +1120,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1098,10 +1134,10 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1112,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1126,10 +1162,10 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1140,10 +1176,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1154,10 +1190,10 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1168,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1182,10 +1218,10 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>
@@ -1196,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1216,130 +1252,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MQuiz4 and slides for PL
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459A68BB-C41B-F140-B3EE-B2C38A7B601A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC1D9A6-2D5C-4D4E-A564-D0F8C4611231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="3660" windowWidth="32320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="5800" yWindow="1940" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>week</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Reinforcement Learning 2;slides(slides/12_RL_Part2.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
-    <t>Proposition Logic and Logical Agents</t>
-  </si>
-  <si>
     <t>Chp 7.1-7.4</t>
   </si>
   <si>
@@ -311,6 +308,15 @@
   </si>
   <si>
     <t>Chp 7.5</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning 3;video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Proposition Logic and Logical Agentsslides(slides/13_PropLogic.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Quiz 4(mquizzes/mquiz4/mquiz4.php);Quiz3 Retake</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1014,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1033,13 +1039,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1050,13 +1053,16 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1067,10 +1073,13 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1081,10 +1090,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1095,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1108,8 +1117,11 @@
       <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1123,7 +1135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1165,7 +1177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1179,7 +1191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1221,7 +1233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Calendar fixes for PL
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC1D9A6-2D5C-4D4E-A564-D0F8C4611231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B48E5-BCA2-0D4A-B7C6-D45FC6331A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5800" yWindow="1940" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
@@ -313,10 +313,10 @@
     <t>Reinforcement Learning 3;video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
-    <t>Proposition Logic and Logical Agentsslides(slides/13_PropLogic.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
-  </si>
-  <si>
     <t>Quiz 4(mquizzes/mquiz4/mquiz4.php);Quiz3 Retake</t>
+  </si>
+  <si>
+    <t>Proposition Logic and Logical Agents;slides(slides/13_PropLogic.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,13 +1053,13 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
         <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
FOL and Probability slides and cal updates
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B48E5-BCA2-0D4A-B7C6-D45FC6331A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE7DB3-E921-5C48-ABAC-146CCBD79359}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="1940" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="-55980" yWindow="1600" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
   <si>
     <t>week</t>
   </si>
@@ -61,15 +61,9 @@
     <t>MDP</t>
   </si>
   <si>
-    <t>Prob</t>
-  </si>
-  <si>
     <t>Chp 1, Chp 2</t>
   </si>
   <si>
-    <t>FOL, Unification</t>
-  </si>
-  <si>
     <t>FOL Resolution and Chaining</t>
   </si>
   <si>
@@ -304,9 +298,6 @@
     <t>Chp 7.1-7.4</t>
   </si>
   <si>
-    <t>Theorm Proving and Resolution</t>
-  </si>
-  <si>
     <t>Chp 7.5</t>
   </si>
   <si>
@@ -317,6 +308,21 @@
   </si>
   <si>
     <t>Proposition Logic and Logical Agents;slides(slides/13_PropLogic.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Chp 8.1 - 8.2</t>
+  </si>
+  <si>
+    <t>Chp 8.3</t>
+  </si>
+  <si>
+    <t>Theorm Proving and Resolution;slides(slides/14_PropLogic_Part2.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>FOL, Unification;slides(slides/15_FOL_Part1.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Probability Review/Lab</t>
   </si>
 </sst>
 </file>
@@ -686,7 +692,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,13 +737,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -751,16 +757,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -774,16 +780,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -797,16 +803,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -820,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,16 +840,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -857,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -871,16 +877,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -894,13 +900,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
         <v>68</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -914,13 +920,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
         <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -934,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -948,13 +954,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
         <v>80</v>
       </c>
-      <c r="F13" t="s">
-        <v>82</v>
-      </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -968,10 +974,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -985,13 +991,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1005,13 +1011,13 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1025,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1039,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1053,13 +1059,13 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1073,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1090,7 +1096,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>94</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1104,7 +1113,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1132,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1160,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1188,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1202,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1216,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1230,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1244,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1264,130 +1276,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for Lab PA3 and slides
</commit_message>
<xml_diff>
--- a/wwwMolloy/Calendar2021.xlsx
+++ b/wwwMolloy/Calendar2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmolloy/teaching/cs444_AI/AIClass/wwwMolloy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE7DB3-E921-5C48-ABAC-146CCBD79359}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14285D78-14F2-C14C-86AB-51A0F4DDCCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55980" yWindow="1600" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
+    <workbookView xWindow="5960" yWindow="2720" windowWidth="38320" windowHeight="23200" xr2:uid="{C28E0A2C-2912-3945-B836-1EB5CA64C473}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>week</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Chp 1, Chp 2</t>
   </si>
   <si>
-    <t>FOL Resolution and Chaining</t>
-  </si>
-  <si>
-    <t>slack</t>
-  </si>
-  <si>
     <t>HW 3</t>
   </si>
   <si>
@@ -85,21 +79,6 @@
     <t>No Class Semester Break 3</t>
   </si>
   <si>
-    <t>Markov Models</t>
-  </si>
-  <si>
-    <t>Hidden Markov Models</t>
-  </si>
-  <si>
-    <t>Bayes - Representations</t>
-  </si>
-  <si>
-    <t>Bayes - Independence</t>
-  </si>
-  <si>
-    <t>Bayes - Inference</t>
-  </si>
-  <si>
     <t>Bayes - Sampling</t>
   </si>
   <si>
@@ -322,7 +301,31 @@
     <t>FOL, Unification;slides(slides/15_FOL_Part1.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
   </si>
   <si>
-    <t>Probability Review/Lab</t>
+    <t>Exam (Retake 2 MQ)</t>
+  </si>
+  <si>
+    <t>MDP Lab PA3</t>
+  </si>
+  <si>
+    <t>FOL Resolution and Chaining;slides(slides/16_FOL_Part2.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Probability Review/Lab;slides(slides/17_Probability.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Bayes Representations</t>
+  </si>
+  <si>
+    <t>Bayes InClass Lab</t>
+  </si>
+  <si>
+    <t>Bayes - Representations;slides(slides/18_Prob_Reasoning.pdf); video(https://canvas.jmu.edu/courses/1775272/modules)</t>
+  </si>
+  <si>
+    <t>Review of Muddiest Points PA3 work</t>
+  </si>
+  <si>
+    <t>PA 3  (PAs/PA.php?paNumber=3)</t>
   </si>
 </sst>
 </file>
@@ -691,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1542B99F-AEAE-5746-AE3C-5BDDA5FB5C77}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,13 +740,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -757,16 +760,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -780,16 +783,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -803,16 +806,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -826,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -840,16 +843,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
         <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -863,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -877,16 +880,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
         <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -900,13 +903,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,13 +923,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -940,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -954,13 +957,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -974,10 +977,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -991,13 +994,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1011,13 +1014,13 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1031,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1045,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1059,13 +1062,13 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1079,10 +1082,10 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1096,10 +1099,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1130,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1144,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1158,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1172,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1186,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1200,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1214,7 +1217,10 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>89</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1228,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1242,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1256,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1276,130 +1282,130 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>